<commit_message>
General insights and qualitative analysis remains
</commit_message>
<xml_diff>
--- a/wyniki/statistical_tests_results.xlsx
+++ b/wyniki/statistical_tests_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\uczelnia\magister\PRACA DYPLOMOWA\wyniki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558E1868-6551-4CF3-9E99-82A6EC08EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1E898C-E3C0-4297-936A-AB4F6D23DD54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="708" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Normality_Results" sheetId="1" r:id="rId1"/>
@@ -152,6 +152,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,11 +204,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -510,12 +514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -563,10 +564,10 @@
         <v>0.11269343644380569</v>
       </c>
       <c r="F2">
-        <v>0.89169299602508545</v>
+        <v>0.89169317483901978</v>
       </c>
       <c r="G2">
-        <v>2.889345400035381E-2</v>
+        <v>2.8893610462546349E-2</v>
       </c>
       <c r="H2">
         <v>0.83567214012145996</v>
@@ -580,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>0.92305374145507813</v>
+        <v>0.92305392026901245</v>
       </c>
       <c r="C3">
-        <v>0.2432373911142349</v>
+        <v>0.24323886632919309</v>
       </c>
       <c r="D3">
         <v>0.88099491596221924</v>
@@ -615,10 +616,10 @@
         <v>2.614805847406387E-2</v>
       </c>
       <c r="D4">
-        <v>0.88559794425964355</v>
+        <v>0.88559812307357788</v>
       </c>
       <c r="E4">
-        <v>6.9872260093688965E-2</v>
+        <v>6.9872625172138214E-2</v>
       </c>
       <c r="F4">
         <v>0.7927168607711792</v>
@@ -650,10 +651,10 @@
         <v>1.477138698101044E-2</v>
       </c>
       <c r="F5">
-        <v>0.85639095306396484</v>
+        <v>0.85639059543609619</v>
       </c>
       <c r="G5">
-        <v>6.833766121417284E-3</v>
+        <v>6.833657156676054E-3</v>
       </c>
       <c r="H5">
         <v>0.72818589210510254</v>
@@ -667,10 +668,10 @@
         <v>13</v>
       </c>
       <c r="B6">
-        <v>0.84110522270202637</v>
+        <v>0.84110546112060547</v>
       </c>
       <c r="C6">
-        <v>1.6855483874678608E-2</v>
+        <v>1.6855573281645771E-2</v>
       </c>
       <c r="D6">
         <v>0.90347498655319214</v>
@@ -714,10 +715,10 @@
         <v>6.2507316470146179E-3</v>
       </c>
       <c r="H7">
-        <v>0.84225296974182129</v>
+        <v>0.84225279092788696</v>
       </c>
       <c r="I7">
-        <v>3.9640055038034916E-3</v>
+        <v>3.9639859460294247E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -766,10 +767,10 @@
         <v>1.5045274049043661E-2</v>
       </c>
       <c r="F9">
-        <v>0.82710927724838257</v>
+        <v>0.82710939645767212</v>
       </c>
       <c r="G9">
-        <v>2.2566737607121472E-3</v>
+        <v>2.256682375445962E-3</v>
       </c>
       <c r="H9">
         <v>0.86417734622955322</v>
@@ -789,16 +790,16 @@
         <v>3.4081991761922843E-2</v>
       </c>
       <c r="D10">
-        <v>0.81390666961669922</v>
+        <v>0.81390684843063354</v>
       </c>
       <c r="E10">
-        <v>7.4545056559145451E-3</v>
+        <v>7.4545401148498058E-3</v>
       </c>
       <c r="F10">
-        <v>0.86510241031646729</v>
+        <v>0.86510264873504639</v>
       </c>
       <c r="G10">
-        <v>9.6478508785367012E-3</v>
+        <v>9.6479486674070358E-3</v>
       </c>
       <c r="H10">
         <v>0.91722977161407471</v>
@@ -841,10 +842,10 @@
         <v>19</v>
       </c>
       <c r="B12">
-        <v>0.86701571941375732</v>
+        <v>0.86701583862304688</v>
       </c>
       <c r="C12">
-        <v>3.8109485059976578E-2</v>
+        <v>3.8109641522169113E-2</v>
       </c>
       <c r="D12">
         <v>0.90897154808044434</v>
@@ -853,10 +854,10 @@
         <v>0.1522577106952667</v>
       </c>
       <c r="F12">
-        <v>0.85951775312423706</v>
+        <v>0.85951763391494751</v>
       </c>
       <c r="G12">
-        <v>7.7278651297092438E-3</v>
+        <v>7.7278297394514084E-3</v>
       </c>
       <c r="H12">
         <v>0.90223866701126099</v>
@@ -870,22 +871,22 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>0.92419660091400146</v>
+        <v>0.92419636249542236</v>
       </c>
       <c r="C13">
-        <v>0.25255650281906128</v>
+        <v>0.25255483388900762</v>
       </c>
       <c r="D13">
-        <v>0.84203433990478516</v>
+        <v>0.84203445911407471</v>
       </c>
       <c r="E13">
-        <v>1.734462566673756E-2</v>
+        <v>1.7344687134027481E-2</v>
       </c>
       <c r="F13">
-        <v>0.78874790668487549</v>
+        <v>0.78874766826629639</v>
       </c>
       <c r="G13">
-        <v>5.8990804245695472E-4</v>
+        <v>5.8990460820496082E-4</v>
       </c>
       <c r="H13">
         <v>0.89332783222198486</v>
@@ -911,10 +912,10 @@
         <v>1.42111349850893E-2</v>
       </c>
       <c r="F14">
-        <v>0.80984163284301758</v>
+        <v>0.80984175205230713</v>
       </c>
       <c r="G14">
-        <v>1.2158514000475411E-3</v>
+        <v>1.215857220813632E-3</v>
       </c>
       <c r="H14">
         <v>0.86124396324157715</v>
@@ -940,16 +941,16 @@
         <v>4.877842590212822E-2</v>
       </c>
       <c r="F15">
-        <v>0.89029514789581299</v>
+        <v>0.89029496908187866</v>
       </c>
       <c r="G15">
-        <v>2.723022177815437E-2</v>
+        <v>2.723001129925251E-2</v>
       </c>
       <c r="H15">
         <v>0.86494624614715576</v>
       </c>
       <c r="I15">
-        <v>9.5877721905708313E-3</v>
+        <v>9.5877842977643013E-3</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -969,10 +970,10 @@
         <v>9.9874779582023621E-2</v>
       </c>
       <c r="F16">
-        <v>0.7455672025680542</v>
+        <v>0.74556714296340942</v>
       </c>
       <c r="G16">
-        <v>1.481379731558263E-4</v>
+        <v>1.4813755115028471E-4</v>
       </c>
       <c r="H16">
         <v>0.89584004878997803</v>
@@ -1021,10 +1022,10 @@
         <v>8.9761149138212204E-3</v>
       </c>
       <c r="D18">
-        <v>0.85528266429901123</v>
+        <v>0.85528254508972168</v>
       </c>
       <c r="E18">
-        <v>2.6219235733151439E-2</v>
+        <v>2.6219135150313381E-2</v>
       </c>
       <c r="F18">
         <v>0.83993721008300781</v>
@@ -1056,16 +1057,16 @@
         <v>6.9449253380298615E-2</v>
       </c>
       <c r="F19">
-        <v>0.87606257200241089</v>
+        <v>0.87606239318847656</v>
       </c>
       <c r="G19">
-        <v>1.504165306687355E-2</v>
+        <v>1.5041562728583809E-2</v>
       </c>
       <c r="H19">
-        <v>0.87546318769454956</v>
+        <v>0.87546300888061523</v>
       </c>
       <c r="I19">
-        <v>1.4676441438496109E-2</v>
+        <v>1.4676352962851519E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1079,10 +1080,10 @@
         <v>3.4114914014935489E-3</v>
       </c>
       <c r="D20">
-        <v>0.74441921710968018</v>
+        <v>0.7444191575050354</v>
       </c>
       <c r="E20">
-        <v>1.1095067020505671E-3</v>
+        <v>1.1095058871433141E-3</v>
       </c>
       <c r="F20">
         <v>0.84956085681915283</v>
@@ -1572,9 +1573,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1594,8 +1602,8 @@
       <c r="B2">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>0.13166801602281419</v>
+      <c r="C2" s="2">
+        <v>0.1520926324815797</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1605,8 +1613,8 @@
       <c r="B3">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>0.67884529942431826</v>
+      <c r="C3" s="2">
+        <v>0.78252792474006738</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1616,8 +1624,8 @@
       <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>0.33399825582199788</v>
+      <c r="C4" s="2">
+        <v>0.40762594770278088</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1627,8 +1635,8 @@
       <c r="B5">
         <v>1.5</v>
       </c>
-      <c r="C5">
-        <v>2.9624447302694329E-3</v>
+      <c r="C5" s="2">
+        <v>3.3680111449411539E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1638,8 +1646,8 @@
       <c r="B6">
         <v>0</v>
       </c>
-      <c r="C6">
-        <v>9.6538748156927215E-3</v>
+      <c r="C6" s="2">
+        <v>1.1866216879384949E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1649,8 +1657,8 @@
       <c r="B7">
         <v>6.5</v>
       </c>
-      <c r="C7">
-        <v>0.78252792474006738</v>
+      <c r="C7" s="2">
+        <v>0.89023005494349738</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1660,8 +1668,8 @@
       <c r="B8">
         <v>10.5</v>
       </c>
-      <c r="C8">
-        <v>0.54612101177706518</v>
+      <c r="C8" s="2">
+        <v>0.60490715489275892</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1671,8 +1679,8 @@
       <c r="B9">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>0.60287820264384251</v>
+      <c r="C9" s="2">
+        <v>0.66461162954100628</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1682,8 +1690,8 @@
       <c r="B10">
         <v>1.5</v>
       </c>
-      <c r="C10">
-        <v>0.41421617824252521</v>
+      <c r="C10" s="2">
+        <v>0.58621368107313998</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,8 +1701,8 @@
       <c r="B11">
         <v>6.5</v>
       </c>
-      <c r="C11">
-        <v>0.78252792474006738</v>
+      <c r="C11" s="2">
+        <v>0.89023005494349738</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,8 +1712,8 @@
       <c r="B12">
         <v>18</v>
       </c>
-      <c r="C12">
-        <v>0.58177691659062281</v>
+      <c r="C12" s="2">
+        <v>0.62442260383854364</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1715,8 +1723,8 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13">
-        <v>2.5239078018325211E-2</v>
+      <c r="C13" s="2">
+        <v>3.1424346521782533E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1726,8 +1734,8 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
-        <v>5.8781721355358862E-2</v>
+      <c r="C14" s="2">
+        <v>8.8973011701813334E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,8 +1745,8 @@
       <c r="B15">
         <v>9</v>
       </c>
-      <c r="C15">
-        <v>0.74773016462413466</v>
+      <c r="C15" s="2">
+        <v>0.83021759177786336</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,8 +1756,8 @@
       <c r="B16">
         <v>5</v>
       </c>
-      <c r="C16">
-        <v>6.5653798087269413E-2</v>
+      <c r="C16" s="2">
+        <v>7.6730336987448799E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1759,8 +1767,8 @@
       <c r="B17">
         <v>14.5</v>
       </c>
-      <c r="C17">
-        <v>0.61797006515962383</v>
+      <c r="C17" s="2">
+        <v>0.669028074498903</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1770,8 +1778,8 @@
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>0.65472084601857694</v>
+      <c r="C18" s="2">
+        <v>0.76559448399576402</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1781,7 +1789,7 @@
       <c r="B19">
         <v>10.5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>1</v>
       </c>
     </row>
@@ -1792,8 +1800,8 @@
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20">
-        <v>0.5637028616507731</v>
+      <c r="C20" s="2">
+        <v>0.77282999268444752</v>
       </c>
     </row>
   </sheetData>
@@ -1805,9 +1813,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1827,8 +1842,8 @@
       <c r="B2">
         <v>12.5</v>
       </c>
-      <c r="C2">
-        <v>6.0617126768370687E-2</v>
+      <c r="C2" s="2">
+        <v>6.7172958725004298E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1838,8 +1853,8 @@
       <c r="B3">
         <v>27.5</v>
       </c>
-      <c r="C3">
-        <v>0.18406848750477081</v>
+      <c r="C3" s="2">
+        <v>0.19655330119230929</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1849,8 +1864,8 @@
       <c r="B4">
         <v>21</v>
       </c>
-      <c r="C4">
-        <v>0.49914362067699453</v>
+      <c r="C4" s="2">
+        <v>0.53272590644282347</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1860,8 +1875,8 @@
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1.9983829447578721E-3</v>
+      <c r="C5" s="2">
+        <v>2.281937253315448E-3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1871,8 +1886,8 @@
       <c r="B6">
         <v>19.5</v>
       </c>
-      <c r="C6">
-        <v>0.71270185665817842</v>
+      <c r="C6" s="2">
+        <v>0.7589513020672245</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1882,8 +1897,8 @@
       <c r="B7">
         <v>41.5</v>
       </c>
-      <c r="C7">
-        <v>0.77509696219598467</v>
+      <c r="C7" s="2">
+        <v>0.8025873486341526</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1893,8 +1908,8 @@
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>5.7805611748857247E-2</v>
+      <c r="C8" s="2">
+        <v>6.6362066456708876E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1904,8 +1919,8 @@
       <c r="B9">
         <v>25</v>
       </c>
-      <c r="C9">
-        <v>0.24881578045962949</v>
+      <c r="C9" s="2">
+        <v>0.26611935562031019</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1915,8 +1930,8 @@
       <c r="B10">
         <v>22.5</v>
       </c>
-      <c r="C10">
-        <v>0.17899240543729039</v>
+      <c r="C10" s="2">
+        <v>0.19252671718116021</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1926,8 +1941,8 @@
       <c r="B11">
         <v>22.5</v>
       </c>
-      <c r="C11">
-        <v>0.59942627929586356</v>
+      <c r="C11" s="2">
+        <v>0.63642497301956835</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1937,8 +1952,8 @@
       <c r="B12">
         <v>28</v>
       </c>
-      <c r="C12">
-        <v>0.65061296393275359</v>
+      <c r="C12" s="2">
+        <v>0.68355287527265496</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1948,8 +1963,8 @@
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13">
-        <v>2.055376150358831E-2</v>
+      <c r="C13" s="2">
+        <v>2.3536373622090701E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1959,8 +1974,8 @@
       <c r="B14">
         <v>20</v>
       </c>
-      <c r="C14">
-        <v>0.40538055645894228</v>
+      <c r="C14" s="2">
+        <v>0.43740644290235942</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1970,8 +1985,8 @@
       <c r="B15">
         <v>20</v>
       </c>
-      <c r="C15">
-        <v>0.21827212208517199</v>
+      <c r="C15" s="2">
+        <v>0.2364984548439383</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1981,8 +1996,8 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16">
-        <v>6.9153204051715716E-3</v>
+      <c r="C16" s="2">
+        <v>7.9101778825628969E-3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1992,8 +2007,8 @@
       <c r="B17">
         <v>34.5</v>
       </c>
-      <c r="C17">
-        <v>0.71398579566938203</v>
+      <c r="C17" s="2">
+        <v>0.74458688845732768</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -2003,8 +2018,8 @@
       <c r="B18">
         <v>6</v>
       </c>
-      <c r="C18">
-        <v>2.6183648097068728E-2</v>
+      <c r="C18" s="2">
+        <v>2.9873144019229029E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2014,8 +2029,8 @@
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19">
-        <v>0.22219460822417109</v>
+      <c r="C19" s="2">
+        <v>0.24295250731663051</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -2025,8 +2040,8 @@
       <c r="B20">
         <v>21</v>
       </c>
-      <c r="C20">
-        <v>0.49021408469758149</v>
+      <c r="C20" s="2">
+        <v>0.52419397534258827</v>
       </c>
     </row>
   </sheetData>
@@ -2038,9 +2053,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2060,7 +2082,7 @@
       <c r="B2">
         <v>133</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>0.81571705431893127</v>
       </c>
     </row>
@@ -2071,7 +2093,7 @@
       <c r="B3">
         <v>118</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.44044718505026131</v>
       </c>
     </row>
@@ -2082,7 +2104,7 @@
       <c r="B4">
         <v>121</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.50337266280192039</v>
       </c>
     </row>
@@ -2093,7 +2115,7 @@
       <c r="B5">
         <v>58.5</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>3.580807488708706E-3</v>
       </c>
     </row>
@@ -2104,7 +2126,7 @@
       <c r="B6">
         <v>77</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>2.3146677790006089E-2</v>
       </c>
     </row>
@@ -2115,7 +2137,7 @@
       <c r="B7">
         <v>112</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.32319458520867561</v>
       </c>
     </row>
@@ -2126,7 +2148,7 @@
       <c r="B8">
         <v>154.5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.61057648906694295</v>
       </c>
     </row>
@@ -2137,7 +2159,7 @@
       <c r="B9">
         <v>106</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.22676807798819529</v>
       </c>
     </row>
@@ -2148,7 +2170,7 @@
       <c r="B10">
         <v>115.5</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>0.38935107580107498</v>
       </c>
     </row>
@@ -2159,7 +2181,7 @@
       <c r="B11">
         <v>106.5</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.23743827413021831</v>
       </c>
     </row>
@@ -2170,7 +2192,7 @@
       <c r="B12">
         <v>133.5</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.82905764542818838</v>
       </c>
     </row>
@@ -2181,7 +2203,7 @@
       <c r="B13">
         <v>84.5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>4.4331113002149258E-2</v>
       </c>
     </row>
@@ -2192,7 +2214,7 @@
       <c r="B14">
         <v>120.5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>0.49254212630875288</v>
       </c>
     </row>
@@ -2203,7 +2225,7 @@
       <c r="B15">
         <v>123</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.55200169359133111</v>
       </c>
     </row>
@@ -2214,7 +2236,7 @@
       <c r="B16">
         <v>107</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.2196311085648891</v>
       </c>
     </row>
@@ -2225,7 +2247,7 @@
       <c r="B17">
         <v>97.5</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>0.12926151383399781</v>
       </c>
     </row>
@@ -2236,7 +2258,7 @@
       <c r="B18">
         <v>129.5</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>0.71913267155375538</v>
       </c>
     </row>
@@ -2247,7 +2269,7 @@
       <c r="B19">
         <v>119.5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.47398608621887028</v>
       </c>
     </row>
@@ -2258,7 +2280,7 @@
       <c r="B20">
         <v>102</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>0.17540668117637589</v>
       </c>
     </row>
@@ -2271,9 +2293,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2293,7 +2322,7 @@
       <c r="B2">
         <v>77</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2.4566117628591171E-2</v>
       </c>
     </row>
@@ -2304,7 +2333,7 @@
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.1542958970586773</v>
       </c>
     </row>
@@ -2315,7 +2344,7 @@
       <c r="B4">
         <v>123.5</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>0.56683752016384803</v>
       </c>
     </row>
@@ -2326,7 +2355,7 @@
       <c r="B5">
         <v>221</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>3.52180467710741E-3</v>
       </c>
     </row>
@@ -2337,7 +2366,7 @@
       <c r="B6">
         <v>133.5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.8285934668760635</v>
       </c>
     </row>
@@ -2348,7 +2377,7 @@
       <c r="B7">
         <v>101</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>0.16701567516969471</v>
       </c>
     </row>
@@ -2359,7 +2388,7 @@
       <c r="B8">
         <v>138.5</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>0.97125944104260442</v>
       </c>
     </row>
@@ -2370,7 +2399,7 @@
       <c r="B9">
         <v>95</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
         <v>0.110132836739304</v>
       </c>
     </row>
@@ -2381,7 +2410,7 @@
       <c r="B10">
         <v>85</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>5.1135177162564549E-2</v>
       </c>
     </row>
@@ -2392,7 +2421,7 @@
       <c r="B11">
         <v>107</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>0.2419681340893963</v>
       </c>
     </row>
@@ -2403,7 +2432,7 @@
       <c r="B12">
         <v>159</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>0.50424146962934868</v>
       </c>
     </row>
@@ -2414,7 +2443,7 @@
       <c r="B13">
         <v>88</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2">
         <v>6.4085352199697174E-2</v>
       </c>
     </row>
@@ -2425,7 +2454,7 @@
       <c r="B14">
         <v>92.5</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
         <v>8.9762518861902341E-2</v>
       </c>
     </row>
@@ -2436,7 +2465,7 @@
       <c r="B15">
         <v>106</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.22140102066900849</v>
       </c>
     </row>
@@ -2447,7 +2476,7 @@
       <c r="B16">
         <v>113.5</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="2">
         <v>0.35202829904975091</v>
       </c>
     </row>
@@ -2458,7 +2487,7 @@
       <c r="B17">
         <v>72.5</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="2">
         <v>1.525211165194254E-2</v>
       </c>
     </row>
@@ -2469,7 +2498,7 @@
       <c r="B18">
         <v>84.5</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>4.8174176305889778E-2</v>
       </c>
     </row>
@@ -2480,7 +2509,7 @@
       <c r="B19">
         <v>105.5</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="2">
         <v>0.22192650577587711</v>
       </c>
     </row>
@@ -2491,7 +2520,7 @@
       <c r="B20">
         <v>87.5</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="2">
         <v>6.1754227954872357E-2</v>
       </c>
     </row>

</xml_diff>